<commit_message>
Push correct working code to addvlast
</commit_message>
<xml_diff>
--- a/mc input.xlsx
+++ b/mc input.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72118EA8-CDAF-4D02-9BED-FBEF2FCFB783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve"> drawing_number</t>
+    <t>Drawing Number</t>
   </si>
   <si>
-    <t xml:space="preserve"> sap_id</t>
+    <t>SAP ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +84,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -280,7 +279,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
@@ -289,7 +288,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
@@ -314,9 +313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,9 +353,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,7 +390,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -426,7 +425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,16 +598,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>34523</v>
       </c>
@@ -624,7 +623,7 @@
         <v>6964700</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>34524</v>
       </c>
@@ -632,7 +631,7 @@
         <v>7486200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>34525</v>
       </c>
@@ -640,7 +639,7 @@
         <v>6888300</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>34526</v>
       </c>
@@ -648,7 +647,7 @@
         <v>6888001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>34527</v>
       </c>
@@ -656,7 +655,7 @@
         <v>7046101</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>34528</v>
       </c>
@@ -664,7 +663,7 @@
         <v>6935900</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>34529</v>
       </c>
@@ -672,7 +671,7 @@
         <v>7058300</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>34530</v>
       </c>
@@ -680,7 +679,7 @@
         <v>7058400</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>34531</v>
       </c>
@@ -688,7 +687,7 @@
         <v>6952700</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>34532</v>
       </c>
@@ -696,7 +695,7 @@
         <v>6943400</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>34533</v>
       </c>
@@ -704,7 +703,7 @@
         <v>6948900</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>34534</v>
       </c>
@@ -712,7 +711,7 @@
         <v>6943800</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>34535</v>
       </c>
@@ -720,7 +719,7 @@
         <v>2466200</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>34536</v>
       </c>
@@ -728,7 +727,7 @@
         <v>2698300</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>34537</v>
       </c>
@@ -736,7 +735,7 @@
         <v>6901600</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>34538</v>
       </c>
@@ -744,7 +743,7 @@
         <v>6925700</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>34539</v>
       </c>
@@ -752,7 +751,7 @@
         <v>6832500</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>34540</v>
       </c>
@@ -760,7 +759,7 @@
         <v>6843900</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>34541</v>
       </c>
@@ -768,7 +767,7 @@
         <v>7005200</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>34542</v>
       </c>
@@ -776,7 +775,7 @@
         <v>6832500</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>34543</v>
       </c>
@@ -784,7 +783,7 @@
         <v>6843900</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>34544</v>
       </c>
@@ -792,7 +791,7 @@
         <v>6920800</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>34545</v>
       </c>
@@ -800,7 +799,7 @@
         <v>6832500</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>34546</v>
       </c>
@@ -808,7 +807,7 @@
         <v>6843900</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>34547</v>
       </c>
@@ -816,7 +815,7 @@
         <v>7001300</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>34548</v>
       </c>
@@ -824,7 +823,7 @@
         <v>2467501</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>34549</v>
       </c>
@@ -832,7 +831,7 @@
         <v>2468603</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>34550</v>
       </c>

</xml_diff>